<commit_message>
Test cases for menu button
</commit_message>
<xml_diff>
--- a/Project1_E_commerce/Test_Cases/Swag Labs.xlsx
+++ b/Project1_E_commerce/Test_Cases/Swag Labs.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="16212" windowHeight="5808"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="16212" windowHeight="5808" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login Module" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Product List Page" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="101">
   <si>
     <t xml:space="preserve">Tittle: </t>
   </si>
@@ -172,6 +172,215 @@
   </si>
   <si>
     <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>The fuctionality of buttons on Product page</t>
+  </si>
+  <si>
+    <t>Click on menu button when no item 
+selected.</t>
+  </si>
+  <si>
+    <t>Login in and be on the product page.</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Functionality of Menu button.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on the Menu button.</t>
+  </si>
+  <si>
+    <t>Click on menu button when one item 
+selected.</t>
+  </si>
+  <si>
+    <t>Click on menu button when all item 
+selected.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on all items add to cart button.
+4. Click on the Menu button.</t>
+  </si>
+  <si>
+    <t>Side menu should open.</t>
+  </si>
+  <si>
+    <t>Click on menu button when one item is added and removed.</t>
+  </si>
+  <si>
+    <t>Click on menu button when some items are added and the some are removed but not all items are removed.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any item add to cart button.
+4. Click on the Menu button.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any item add to cart button.
+4. Click on that item again to remove the item.
+5. Click on the Menu button.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any 4 item add to cart button.
+4. Click on that 2 item again to remove the item.
+5. Click on the Menu button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Side menu should open.</t>
+  </si>
+  <si>
+    <t>TP-1</t>
+  </si>
+  <si>
+    <t>TP-2</t>
+  </si>
+  <si>
+    <t>TP-3</t>
+  </si>
+  <si>
+    <t>TP-4</t>
+  </si>
+  <si>
+    <t>TP-5</t>
+  </si>
+  <si>
+    <t>Functionality of Cart button.</t>
+  </si>
+  <si>
+    <t>Click on Cart button when no item 
+selected.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on the Cart button.</t>
+  </si>
+  <si>
+    <t>Click on Cart button when one item 
+selected.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any item add to cart button.
+4. Click on the Cart button.</t>
+  </si>
+  <si>
+    <t>Click on Cart button when all item 
+selected.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on all items add to cart button.
+4. Click on the Cart button.</t>
+  </si>
+  <si>
+    <t>Click on Cart button when one item is added and removed.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any item add to cart button.
+4. Click on that item again to remove the item.
+5. Click on the Cart button.</t>
+  </si>
+  <si>
+    <t>Click on Cart button when some items are added and the some are removed but not all items are removed.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on any 4 item add to cart button.
+4. Click on that 2 item again to remove the item.
+5. Click on the Cart button.</t>
+  </si>
+  <si>
+    <t>Cart page should not open.</t>
+  </si>
+  <si>
+    <t>Cart page should open with selected items.</t>
+  </si>
+  <si>
+    <t>TP-6</t>
+  </si>
+  <si>
+    <t>TP-7</t>
+  </si>
+  <si>
+    <t>TP-8</t>
+  </si>
+  <si>
+    <t>TP-9</t>
+  </si>
+  <si>
+    <t>TP-10</t>
+  </si>
+  <si>
+    <t>Functionality of the opening an 
+Item detail.</t>
+  </si>
+  <si>
+    <t>Open details of item when item is not 
+added to cart.</t>
+  </si>
+  <si>
+    <t>Open details of item when item is added to the cart.</t>
+  </si>
+  <si>
+    <t>Open details of item when item is added to the cart and then removed.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3. Click on image of item.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3.Click on Add to cart button.
+4. Click on image of item.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3.Click on Add to cart button.
+4.Click on same item remove button.
+5. Click on image of item.</t>
+  </si>
+  <si>
+    <t>Open details of item when item is not added to the cart but any other item is added to the cart.</t>
+  </si>
+  <si>
+    <t>Login in and be on the product page and
+ a item is added to the cart.</t>
+  </si>
+  <si>
+    <t>1. Login the account.
+2. Product page open.
+3.Click on Add to cart button of an item.
+5. Click on image of item not added to cart.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Functionality of 'Add to cart button'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click </t>
   </si>
 </sst>
 </file>
@@ -213,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -339,11 +548,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,6 +594,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -378,19 +629,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -710,107 +957,107 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1"/>
     <row r="9" spans="1:12">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="23"/>
+      <c r="H9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="20" t="s">
         <v>17</v>
       </c>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1">
       <c r="A10" s="17"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="13"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:12" ht="43.2">
       <c r="A11" s="7" t="s">
@@ -1030,127 +1277,133 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="21"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="20"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="20"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="21"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="20"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="20"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="21"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="20"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="22"/>
+      <c r="A27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -1158,15 +1411,9 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1175,12 +1422,404 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1"/>
+    <row r="8" spans="1:10">
+      <c r="A8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="A9" s="17"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" ht="43.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="72">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="100.8">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="100.8">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="72">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="72">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="100.8">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="100.8">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2">
+      <c r="B20" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="57.6">
+      <c r="C21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="86.4">
+      <c r="C22" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="86.4">
+      <c r="C23" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>